<commit_message>
update Lighthouse test results (add t-test for FCP,LCP and Speed Index)
</commit_message>
<xml_diff>
--- a/lighthouse-test/Lighthouse Ergebnisse.xlsx
+++ b/lighthouse-test/Lighthouse Ergebnisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aramfilak/Desktop/bachelorarbeit-blog-prototyp/lighthouse-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{719ACB72-9CEC-4F41-A665-80E15C9BA65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C6FDE59-8CB6-9541-A520-AE09E0D01A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30060" yWindow="520" windowWidth="30100" windowHeight="33340" xr2:uid="{0471C796-84F1-154D-A24D-95E026A53E39}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{0471C796-84F1-154D-A24D-95E026A53E39}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Test_Ergebnisse(1)" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
   <si>
     <t>Anwendung</t>
   </si>
@@ -163,12 +163,69 @@
   <si>
     <t>Min</t>
   </si>
+  <si>
+    <t>FCP React</t>
+  </si>
+  <si>
+    <t>FCP Next.js</t>
+  </si>
+  <si>
+    <t>LCP React</t>
+  </si>
+  <si>
+    <t>LCP Next.js</t>
+  </si>
+  <si>
+    <t>Speed Index React</t>
+  </si>
+  <si>
+    <t>Speed Index Next.js</t>
+  </si>
+  <si>
+    <t>Mittelwert</t>
+  </si>
+  <si>
+    <t>t-Test unter der Annahme gleicher Varianzen</t>
+  </si>
+  <si>
+    <t>Varianz</t>
+  </si>
+  <si>
+    <t>Beobachtungen</t>
+  </si>
+  <si>
+    <t>Gepoolte Varianz</t>
+  </si>
+  <si>
+    <t>Hypothetische Differenz der Mittelwerte</t>
+  </si>
+  <si>
+    <t>Freiheitsgrade (df)</t>
+  </si>
+  <si>
+    <t>t-Statistik</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) einseitig</t>
+  </si>
+  <si>
+    <t>Kritischer t-Wert bei einseitigem t-Test</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) zweiseitig</t>
+  </si>
+  <si>
+    <t>Kritischer t-Wert bei zweiseitigem t-Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,6 +369,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -649,6 +714,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -694,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -708,6 +793,13 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1083,16 +1175,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9406313-36E5-EF40-BDDD-ABB4119D46DE}">
-  <dimension ref="A1:AA58"/>
+  <dimension ref="A1:CC119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="W63" sqref="W63"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="185" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" customWidth="1"/>
     <col min="25" max="25" width="21.33203125" customWidth="1"/>
   </cols>
@@ -5007,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
@@ -5089,7 +5182,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -5169,7 +5262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:81" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
@@ -5249,7 +5342,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>36</v>
@@ -5333,7 +5426,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
@@ -5415,7 +5508,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4" t="s">
@@ -5497,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
@@ -5577,7 +5670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4" t="s">
@@ -5659,7 +5752,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
@@ -5739,7 +5832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
@@ -5818,6 +5911,1845 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
+    </row>
+    <row r="63" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="P63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="S63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="U63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="V63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="W63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="X63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Y63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Z63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AC63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AD63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AE63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AF63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AG63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AH63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AI63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AJ63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AK63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AL63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AM63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AN63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AO63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AP63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AQ63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AR63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AS63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AT63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AU63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AV63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AW63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AX63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AY63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AZ63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="BA63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BB63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BC63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BD63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BE63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BF63" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BG63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BH63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BI63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BJ63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BK63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BL63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BM63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BN63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BO63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BP63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BQ63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BR63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BS63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BT63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BU63" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BV63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BW63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BX63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BY63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BZ63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="CA63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="CB63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="CC63" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="N64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="O64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="P64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="S64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="T64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="U64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="V64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="W64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="X64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Y64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Z64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AA64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AB64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AC64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AD64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AE64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AF64" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AG64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AH64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AI64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AJ64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AK64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AL64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AM64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="AN64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AO64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AP64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AQ64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AR64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AS64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AT64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AU64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AV64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AW64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AX64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AY64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AZ64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BA64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BB64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BC64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BD64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BE64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BF64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BG64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BH64" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BI64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BJ64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BK64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BL64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BM64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BN64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BO64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BP64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BQ64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BR64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BS64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BT64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BU64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BV64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BW64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BX64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BY64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BZ64" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="CA64" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="CB64" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="CC64" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="D69" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="16">
+        <v>0.22405063291139221</v>
+      </c>
+      <c r="D70" s="13">
+        <v>0.23544303797468347</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B71" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="16">
+        <v>4.4141512495943962E-3</v>
+      </c>
+      <c r="D71" s="13">
+        <v>1.436871145731904E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="16">
+        <v>79</v>
+      </c>
+      <c r="D72" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="16">
+        <v>9.3914313534567175E-3</v>
+      </c>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="16">
+        <v>0</v>
+      </c>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="16">
+        <v>156</v>
+      </c>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B76" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="16">
+        <v>-0.7388360397433571</v>
+      </c>
+      <c r="D76" s="13"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B77" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="16">
+        <v>0.23055836936363838</v>
+      </c>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" s="16">
+        <v>1.654679995671714</v>
+      </c>
+      <c r="D78" s="13"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="16">
+        <v>0.46111673872727676</v>
+      </c>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" s="17">
+        <v>1.9752875077034502</v>
+      </c>
+      <c r="D80" s="14"/>
+    </row>
+    <row r="83" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="L83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="M83" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="O83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="R83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="S83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="T83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="U83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="V83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="W83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="X83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="Y83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="Z83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="AA83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="AB83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AC83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AD83" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AE83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AF83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AG83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AH83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AI83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AJ83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AK83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AL83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AM83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="AN83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AO83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AP83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AQ83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AR83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AS83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AT83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AU83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AV83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AW83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AX83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AY83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AZ83" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="BA83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BB83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BC83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BD83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BE83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BF83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BG83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BH83" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BI83" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BJ83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BK83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BL83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BM83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BN83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BO83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BP83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BQ83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BR83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BS83" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="BT83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BU83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BV83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BW83" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="BX83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BY83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BZ83" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="CA83" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="CB83" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="CC83" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="H84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="J84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="L84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="M84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="P84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="S84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="T84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="U84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="V84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="X84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Y84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Z84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AA84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AB84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AC84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AD84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AE84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AF84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AG84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AH84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AI84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AJ84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AK84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AL84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AM84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="AN84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AO84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AP84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AQ84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AR84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AS84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AT84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AU84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AV84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AW84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AX84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AY84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AZ84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BA84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BB84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BC84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BD84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BE84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BF84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BG84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BH84" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="BI84" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BJ84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BK84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BL84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BM84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="BN84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BO84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BP84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BQ84" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="BR84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BS84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BT84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BU84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BV84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BW84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BX84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BY84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BZ84" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="CA84" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="CB84" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="CC84" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B89" s="15"/>
+      <c r="C89" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="D89" s="15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B90" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C90" s="13">
+        <v>0.55822784810126613</v>
+      </c>
+      <c r="D90" s="13">
+        <v>0.27468354430379727</v>
+      </c>
+    </row>
+    <row r="91" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C91" s="13">
+        <v>3.8873742291463044E-2</v>
+      </c>
+      <c r="D91" s="13">
+        <v>2.0889321648815382E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B92" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" s="13">
+        <v>79</v>
+      </c>
+      <c r="D92" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B93" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="13">
+        <v>2.9881531970139211E-2</v>
+      </c>
+      <c r="D93" s="13"/>
+    </row>
+    <row r="94" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B94" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" s="13">
+        <v>0</v>
+      </c>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B95" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95" s="13">
+        <v>156</v>
+      </c>
+      <c r="D95" s="13"/>
+    </row>
+    <row r="96" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B96" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" s="13">
+        <v>10.309035740045536</v>
+      </c>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B97" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C97" s="13">
+        <v>1.2485053150542021E-19</v>
+      </c>
+      <c r="D97" s="13"/>
+    </row>
+    <row r="98" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B98" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C98" s="13">
+        <v>1.654679995671714</v>
+      </c>
+      <c r="D98" s="13"/>
+    </row>
+    <row r="99" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B99" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" s="13">
+        <v>2.4970106301084042E-19</v>
+      </c>
+      <c r="D99" s="13"/>
+    </row>
+    <row r="100" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C100" s="14">
+        <v>1.9752875077034502</v>
+      </c>
+      <c r="D100" s="14"/>
+    </row>
+    <row r="103" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>47</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="M103" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="O103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="P103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="R103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="S103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="T103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="U103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="V103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="W103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="X103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="Y103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="Z103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AA103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AB103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AC103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AD103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AE103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AF103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AG103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AH103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AI103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AJ103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AK103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AL103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AM103" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AN103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AO103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AP103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AQ103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AR103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AS103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AT103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AU103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AV103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AW103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AX103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AY103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AZ103" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="BA103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BB103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BC103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BD103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BE103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BF103" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BG103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BH103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BI103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BJ103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BK103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BL103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BM103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BN103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BO103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BP103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BQ103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BR103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BS103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BT103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BU103" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="BV103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BW103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BX103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BY103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BZ103" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="CA103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="CB103" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="CC103" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M104" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="O104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="P104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="S104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="T104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="U104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="V104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="W104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="X104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Y104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Z104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AA104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AB104" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AC104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AD104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AE104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AF104" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AG104" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AH104" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AI104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AJ104" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AK104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AL104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AM104" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AN104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AO104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AP104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AQ104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AR104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AS104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AT104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AU104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AV104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AW104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AX104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AY104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AZ104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BA104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BB104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BC104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BD104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BE104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BF104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BG104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BH104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BI104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="BJ104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BK104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BL104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BM104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BN104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BO104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BP104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BQ104" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="BR104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BS104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BT104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="BU104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BV104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BW104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BX104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BY104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="BZ104" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="CA104" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="CB104" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="CC104" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B108" s="15"/>
+      <c r="C108" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="D108" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B109" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C109" s="13">
+        <v>0.32531645569620271</v>
+      </c>
+      <c r="D109" s="13">
+        <v>0.22911392405063283</v>
+      </c>
+    </row>
+    <row r="110" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B110" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C110" s="13">
+        <v>8.5816293411229028E-3</v>
+      </c>
+      <c r="D110" s="13">
+        <v>1.5936384290814606E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B111" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C111" s="13">
+        <v>79</v>
+      </c>
+      <c r="D111" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="112" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="B112" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" s="13">
+        <v>1.2259006815968755E-2</v>
+      </c>
+      <c r="D112" s="13"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B113" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C113" s="13">
+        <v>0</v>
+      </c>
+      <c r="D113" s="13"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B114" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="13">
+        <v>156</v>
+      </c>
+      <c r="D114" s="13"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B115" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" s="13">
+        <v>5.4608142666024815</v>
+      </c>
+      <c r="D115" s="13"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B116" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C116" s="13">
+        <v>9.1621741495857466E-8</v>
+      </c>
+      <c r="D116" s="13"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B117" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C117" s="13">
+        <v>1.654679995671714</v>
+      </c>
+      <c r="D117" s="13"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B118" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C118" s="13">
+        <v>1.8324348299171493E-7</v>
+      </c>
+      <c r="D118" s="13"/>
+    </row>
+    <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C119" s="14">
+        <v>1.9752875077034502</v>
+      </c>
+      <c r="D119" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
update Lighthouse test results
</commit_message>
<xml_diff>
--- a/lighthouse-test/Lighthouse Ergebnisse.xlsx
+++ b/lighthouse-test/Lighthouse Ergebnisse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aramfilak/Desktop/bachelorarbeit-blog-prototyp/lighthouse-test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aramfilak/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C6FDE59-8CB6-9541-A520-AE09E0D01A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C95BEC-C9B2-024C-9953-8F32158E748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{0471C796-84F1-154D-A24D-95E026A53E39}"/>
+    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{0471C796-84F1-154D-A24D-95E026A53E39}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Test_Ergebnisse(1)" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
   <si>
     <t>Anwendung</t>
   </si>
@@ -217,14 +217,53 @@
   <si>
     <t>Kritischer t-Wert bei zweiseitigem t-Test</t>
   </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Equal Variances</t>
+  </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Pooled Variance</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-  </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -779,7 +818,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -793,13 +832,12 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1177,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9406313-36E5-EF40-BDDD-ABB4119D46DE}">
   <dimension ref="A1:CC119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="185" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,6 +1224,7 @@
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" customWidth="1"/>
     <col min="25" max="25" width="21.33203125" customWidth="1"/>
   </cols>
@@ -6412,118 +6451,118 @@
       <c r="A69" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="D69" s="15">
-        <v>0.3</v>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="13" t="s">
+      <c r="B70" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="16">
-        <v>0.22405063291139221</v>
-      </c>
-      <c r="D70" s="13">
-        <v>0.23544303797468347</v>
+      <c r="C70" s="14">
+        <v>0.22374999999999981</v>
+      </c>
+      <c r="D70" s="14">
+        <v>0.2362499999999999</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="13" t="s">
+      <c r="B71" t="s">
         <v>51</v>
       </c>
-      <c r="C71" s="16">
-        <v>4.4141512495943962E-3</v>
-      </c>
-      <c r="D71" s="13">
-        <v>1.436871145731904E-2</v>
+      <c r="C71" s="14">
+        <v>4.3655063291140259E-3</v>
+      </c>
+      <c r="D71" s="14">
+        <v>1.4238924050632915E-2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="13" t="s">
+      <c r="B72" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="16">
-        <v>79</v>
-      </c>
-      <c r="D72" s="13">
-        <v>79</v>
+      <c r="C72" s="14">
+        <v>80</v>
+      </c>
+      <c r="D72" s="14">
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B73" s="13" t="s">
+      <c r="B73" t="s">
         <v>53</v>
       </c>
-      <c r="C73" s="16">
-        <v>9.3914313534567175E-3</v>
-      </c>
-      <c r="D73" s="13"/>
+      <c r="C73" s="14">
+        <v>9.3022151898734702E-3</v>
+      </c>
+      <c r="D73" s="14"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B74" s="13" t="s">
+      <c r="B74" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="16">
-        <v>0</v>
-      </c>
-      <c r="D74" s="13"/>
+      <c r="C74" s="14">
+        <v>0</v>
+      </c>
+      <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="13" t="s">
+      <c r="B75" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="16">
-        <v>156</v>
-      </c>
-      <c r="D75" s="13"/>
+      <c r="C75" s="14">
+        <v>158</v>
+      </c>
+      <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="13" t="s">
+      <c r="B76" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="16">
-        <v>-0.7388360397433571</v>
-      </c>
-      <c r="D76" s="13"/>
+      <c r="C76" s="14">
+        <v>-0.8196846791875424</v>
+      </c>
+      <c r="D76" s="14"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="13" t="s">
+      <c r="B77" t="s">
         <v>57</v>
       </c>
-      <c r="C77" s="16">
-        <v>0.23055836936363838</v>
-      </c>
-      <c r="D77" s="13"/>
+      <c r="C77" s="14">
+        <v>0.2068153289229071</v>
+      </c>
+      <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B78" s="13" t="s">
+      <c r="B78" t="s">
         <v>58</v>
       </c>
-      <c r="C78" s="16">
-        <v>1.654679995671714</v>
-      </c>
-      <c r="D78" s="13"/>
+      <c r="C78" s="14">
+        <v>1.654554875439588</v>
+      </c>
+      <c r="D78" s="14"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="13" t="s">
+      <c r="B79" t="s">
         <v>59</v>
       </c>
-      <c r="C79" s="16">
-        <v>0.46111673872727676</v>
-      </c>
-      <c r="D79" s="13"/>
+      <c r="C79" s="14">
+        <v>0.41363065784581421</v>
+      </c>
+      <c r="D79" s="14"/>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C80" s="17">
-        <v>1.9752875077034502</v>
-      </c>
-      <c r="D80" s="14"/>
+      <c r="C80" s="15">
+        <v>1.9750920727120791</v>
+      </c>
+      <c r="D80" s="15"/>
     </row>
     <row r="83" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
@@ -7025,118 +7064,118 @@
     </row>
     <row r="88" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="89" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B89" s="15"/>
-      <c r="C89" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="D89" s="15">
-        <v>0.4</v>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B90" s="13" t="s">
+      <c r="B90" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="13">
-        <v>0.55822784810126613</v>
-      </c>
-      <c r="D90" s="13">
-        <v>0.27468354430379727</v>
+      <c r="C90" s="14">
+        <v>0.55875000000000041</v>
+      </c>
+      <c r="D90" s="14">
+        <v>0.27624999999999977</v>
       </c>
     </row>
     <row r="91" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B91" s="13" t="s">
+      <c r="B91" t="s">
         <v>51</v>
       </c>
-      <c r="C91" s="13">
-        <v>3.8873742291463044E-2</v>
-      </c>
-      <c r="D91" s="13">
-        <v>2.0889321648815382E-2</v>
+      <c r="C91" s="14">
+        <v>3.8403481012657399E-2</v>
+      </c>
+      <c r="D91" s="14">
+        <v>2.0821202531645634E-2</v>
       </c>
     </row>
     <row r="92" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B92" s="13" t="s">
+      <c r="B92" t="s">
         <v>52</v>
       </c>
-      <c r="C92" s="13">
-        <v>79</v>
-      </c>
-      <c r="D92" s="13">
-        <v>79</v>
+      <c r="C92" s="14">
+        <v>80</v>
+      </c>
+      <c r="D92" s="14">
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B93" s="13" t="s">
+      <c r="B93" t="s">
         <v>53</v>
       </c>
-      <c r="C93" s="13">
-        <v>2.9881531970139211E-2</v>
-      </c>
-      <c r="D93" s="13"/>
+      <c r="C93" s="14">
+        <v>2.9612341772151517E-2</v>
+      </c>
+      <c r="D93" s="14"/>
     </row>
     <row r="94" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B94" s="13" t="s">
+      <c r="B94" t="s">
         <v>54</v>
       </c>
-      <c r="C94" s="13">
-        <v>0</v>
-      </c>
-      <c r="D94" s="13"/>
+      <c r="C94" s="14">
+        <v>0</v>
+      </c>
+      <c r="D94" s="14"/>
     </row>
     <row r="95" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B95" s="13" t="s">
+      <c r="B95" t="s">
         <v>55</v>
       </c>
-      <c r="C95" s="13">
-        <v>156</v>
-      </c>
-      <c r="D95" s="13"/>
+      <c r="C95" s="14">
+        <v>158</v>
+      </c>
+      <c r="D95" s="14"/>
     </row>
     <row r="96" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B96" s="13" t="s">
+      <c r="B96" t="s">
         <v>56</v>
       </c>
-      <c r="C96" s="13">
-        <v>10.309035740045536</v>
-      </c>
-      <c r="D96" s="13"/>
+      <c r="C96" s="14">
+        <v>10.382742211327347</v>
+      </c>
+      <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B97" s="13" t="s">
+      <c r="B97" t="s">
         <v>57</v>
       </c>
-      <c r="C97" s="13">
-        <v>1.2485053150542021E-19</v>
-      </c>
-      <c r="D97" s="13"/>
+      <c r="C97" s="14">
+        <v>7.0285039561260385E-20</v>
+      </c>
+      <c r="D97" s="14"/>
     </row>
     <row r="98" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B98" s="13" t="s">
+      <c r="B98" t="s">
         <v>58</v>
       </c>
-      <c r="C98" s="13">
-        <v>1.654679995671714</v>
-      </c>
-      <c r="D98" s="13"/>
+      <c r="C98" s="14">
+        <v>1.654554875439588</v>
+      </c>
+      <c r="D98" s="14"/>
     </row>
     <row r="99" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B99" s="13" t="s">
+      <c r="B99" t="s">
         <v>59</v>
       </c>
-      <c r="C99" s="13">
-        <v>2.4970106301084042E-19</v>
-      </c>
-      <c r="D99" s="13"/>
+      <c r="C99" s="14">
+        <v>1.4057007912252077E-19</v>
+      </c>
+      <c r="D99" s="14"/>
     </row>
     <row r="100" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C100" s="14">
-        <v>1.9752875077034502</v>
-      </c>
-      <c r="D100" s="14"/>
+      <c r="C100" s="15">
+        <v>1.9750920727120791</v>
+      </c>
+      <c r="D100" s="15"/>
     </row>
     <row r="103" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -7633,123 +7672,123 @@
         <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="107" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="108" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B108" s="15"/>
-      <c r="C108" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="D108" s="15">
-        <v>0.3</v>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="109" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B109" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C109" s="13">
-        <v>0.32531645569620271</v>
-      </c>
-      <c r="D109" s="13">
-        <v>0.22911392405063283</v>
+      <c r="B109" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C109" s="14">
+        <v>0.32625000000000015</v>
+      </c>
+      <c r="D109" s="14">
+        <v>0.22999999999999993</v>
       </c>
     </row>
     <row r="110" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B110" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C110" s="13">
-        <v>8.5816293411229028E-3</v>
-      </c>
-      <c r="D110" s="13">
-        <v>1.5936384290814606E-2</v>
+      <c r="B110" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="14">
+        <v>8.5427215189872088E-3</v>
+      </c>
+      <c r="D110" s="14">
+        <v>1.5797468354430313E-2</v>
       </c>
     </row>
     <row r="111" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B111" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C111" s="13">
-        <v>79</v>
-      </c>
-      <c r="D111" s="13">
-        <v>79</v>
+      <c r="B111" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C111" s="14">
+        <v>80</v>
+      </c>
+      <c r="D111" s="14">
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B112" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C112" s="13">
-        <v>1.2259006815968755E-2</v>
-      </c>
-      <c r="D112" s="13"/>
+      <c r="B112" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C112" s="14">
+        <v>1.217009493670876E-2</v>
+      </c>
+      <c r="D112" s="14"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B113" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C113" s="13">
-        <v>0</v>
-      </c>
-      <c r="D113" s="13"/>
+      <c r="B113" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" s="14">
+        <v>0</v>
+      </c>
+      <c r="D113" s="14"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B114" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C114" s="13">
-        <v>156</v>
-      </c>
-      <c r="D114" s="13"/>
+      <c r="B114" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C114" s="14">
+        <v>158</v>
+      </c>
+      <c r="D114" s="14"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B115" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C115" s="13">
-        <v>5.4608142666024815</v>
-      </c>
-      <c r="D115" s="13"/>
+      <c r="B115" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C115" s="14">
+        <v>5.5180261057982802</v>
+      </c>
+      <c r="D115" s="14"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B116" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C116" s="13">
-        <v>9.1621741495857466E-8</v>
-      </c>
-      <c r="D116" s="13"/>
+      <c r="B116" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C116" s="14">
+        <v>6.8749594792438735E-8</v>
+      </c>
+      <c r="D116" s="14"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B117" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C117" s="13">
-        <v>1.654679995671714</v>
-      </c>
-      <c r="D117" s="13"/>
+      <c r="B117" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C117" s="14">
+        <v>1.654554875439588</v>
+      </c>
+      <c r="D117" s="14"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C118" s="13">
-        <v>1.8324348299171493E-7</v>
-      </c>
-      <c r="D118" s="13"/>
+      <c r="B118" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C118" s="14">
+        <v>1.3749918958487747E-7</v>
+      </c>
+      <c r="D118" s="14"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C119" s="14">
-        <v>1.9752875077034502</v>
-      </c>
-      <c r="D119" s="14"/>
+      <c r="B119" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C119" s="15">
+        <v>1.9750920727120791</v>
+      </c>
+      <c r="D119" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>